<commit_message>
update TDD excel files
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966F2A21-D4E5-48B9-B56B-843354DF8F83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156CBFC8-6B4E-461D-A220-93647C6565A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2240" yWindow="2240" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,18 +28,12 @@
     <t>password</t>
   </si>
   <si>
-    <t xml:space="preserve">admin@yourstore.com </t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
     <t>adm</t>
   </si>
   <si>
-    <t>adm@yourstore.com</t>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
@@ -47,13 +41,19 @@
   </si>
   <si>
     <t>exp</t>
+  </si>
+  <si>
+    <t>capexlogin@yopmail.com</t>
+  </si>
+  <si>
+    <t>failcapexloginfail@yopmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,14 +80,6 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="14"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -135,16 +127,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -464,69 +459,69 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:U33"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="4" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>